<commit_message>
Progress on merging P&L programmes
</commit_message>
<xml_diff>
--- a/pnl_pf.xlsx
+++ b/pnl_pf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EYKS\Documents\UNDERGRADUATE\GHOSAL\REPO\P&amp;L CALC, BRINSON PERFORMANCE EVALUATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAA408A-BE0C-4A18-8836-FA49E62324AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13BD671-BF5B-45CD-89B1-8CE3F5355DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1290" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Company name</t>
   </si>
@@ -64,7 +64,7 @@
     <t>USD</t>
   </si>
   <si>
-    <t>USA</t>
+    <t>United States</t>
   </si>
   <si>
     <t>Technology</t>
@@ -76,12 +76,18 @@
     <t>AMZN</t>
   </si>
   <si>
+    <t>Consumer Cyclical</t>
+  </si>
+  <si>
     <t>Alphabet Inc.</t>
   </si>
   <si>
     <t>GOOG</t>
   </si>
   <si>
+    <t>Communication Services</t>
+  </si>
+  <si>
     <t>NVIDIA Corporation</t>
   </si>
   <si>
@@ -100,49 +106,28 @@
     <t>PFE</t>
   </si>
   <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
+    <t>Enphase Energy, Inc.</t>
+  </si>
+  <si>
     <t>ENPH</t>
   </si>
   <si>
+    <t>Cisco Systems, Inc.</t>
+  </si>
+  <si>
     <t>CSCO</t>
   </si>
   <si>
+    <t>Visa Inc.</t>
+  </si>
+  <si>
     <t>V</t>
   </si>
   <si>
-    <t>QCOM</t>
-  </si>
-  <si>
-    <t>TSLA</t>
-  </si>
-  <si>
-    <t>SHEL</t>
-  </si>
-  <si>
-    <t>AZN</t>
-  </si>
-  <si>
-    <t>ULVR</t>
-  </si>
-  <si>
-    <t>HSBA</t>
-  </si>
-  <si>
-    <t>BP</t>
-  </si>
-  <si>
-    <t>LSEG</t>
-  </si>
-  <si>
-    <t>JPM</t>
-  </si>
-  <si>
-    <t>UBSG</t>
-  </si>
-  <si>
-    <t>MSFT</t>
-  </si>
-  <si>
-    <t>LLOY.L</t>
+    <t>Financial Services</t>
   </si>
 </sst>
 </file>
@@ -150,7 +135,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -206,7 +191,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,15 +494,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="17.90625" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -552,7 +541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -560,7 +549,7 @@
         <v>12</v>
       </c>
       <c r="C2">
-        <v>141.80000000000001</v>
+        <v>146.21</v>
       </c>
       <c r="D2">
         <v>133.88</v>
@@ -587,7 +576,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -595,126 +584,156 @@
         <v>17</v>
       </c>
       <c r="C3">
-        <v>92.21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>94.185000000000002</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>100.18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>165.63499999999999</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>28.864999999999998</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>51.02</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>332.63</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9">
+        <v>49.365000000000002</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10">
+        <v>216.01</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10">
         <v>19</v>
-      </c>
-      <c r="C4">
-        <v>96.13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5">
-        <v>158.82429999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6">
-        <v>28.465</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7">
-        <v>49.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>